<commit_message>
generación actividad 1 json
</commit_message>
<xml_diff>
--- a/src/static/cleaned_data/cleaned_data_name.xlsx
+++ b/src/static/cleaned_data/cleaned_data_name.xlsx
@@ -490,19 +490,19 @@
         <v>21000000</v>
       </c>
       <c r="D2" t="n">
-        <v>82760.04437711994</v>
+        <v>82927.52916336917</v>
       </c>
       <c r="E2" t="n">
-        <v>6738130970.06928</v>
+        <v>6787931376.162843</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.954651571863924</v>
+        <v>-1.800994089607436</v>
       </c>
       <c r="G2" t="n">
-        <v>83044.74235883883</v>
+        <v>82979.25552039099</v>
       </c>
       <c r="H2" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="3">
@@ -520,19 +520,19 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1826.045419021544</v>
+        <v>1833.695986101409</v>
       </c>
       <c r="E3" t="n">
-        <v>5501487637.245388</v>
+        <v>5548289274.7092</v>
       </c>
       <c r="F3" t="n">
-        <v>-4.147815923051545</v>
+        <v>-3.790752072379215</v>
       </c>
       <c r="G3" t="n">
-        <v>1849.313034122267</v>
+        <v>1846.805894832743</v>
       </c>
       <c r="H3" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="4">
@@ -550,19 +550,19 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1.003159884327486</v>
+        <v>1.003285359699285</v>
       </c>
       <c r="E4" t="n">
-        <v>21638531272.97508</v>
+        <v>21803680461.65792</v>
       </c>
       <c r="F4" t="n">
-        <v>0.179622143766819</v>
+        <v>0.175187192831505</v>
       </c>
       <c r="G4" t="n">
-        <v>1.000608313705002</v>
+        <v>1.00057496401654</v>
       </c>
       <c r="H4" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="5">
@@ -580,19 +580,19 @@
         <v>100000000000</v>
       </c>
       <c r="D5" t="n">
-        <v>2.133704038873</v>
+        <v>2.147509659614922</v>
       </c>
       <c r="E5" t="n">
-        <v>1621712633.544061</v>
+        <v>1638145769.172129</v>
       </c>
       <c r="F5" t="n">
-        <v>-3.585144538809004</v>
+        <v>-2.969282930273178</v>
       </c>
       <c r="G5" t="n">
-        <v>2.126768482759352</v>
+        <v>2.123485054649936</v>
       </c>
       <c r="H5" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="6">
@@ -610,19 +610,19 @@
         <v>144006830</v>
       </c>
       <c r="D6" t="n">
-        <v>603.2092953755001</v>
+        <v>605.27236425811</v>
       </c>
       <c r="E6" t="n">
-        <v>315523338.8965769</v>
+        <v>316941868.5504553</v>
       </c>
       <c r="F6" t="n">
-        <v>-3.087979783386078</v>
+        <v>-2.630675894687077</v>
       </c>
       <c r="G6" t="n">
-        <v>606.7164538032188</v>
+        <v>606.1983101043919</v>
       </c>
       <c r="H6" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="7">
@@ -640,19 +640,19 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>124.6129436721944</v>
+        <v>125.2021089351357</v>
       </c>
       <c r="E7" t="n">
-        <v>1297320343.954299</v>
+        <v>1311190636.556914</v>
       </c>
       <c r="F7" t="n">
-        <v>-4.102129215447629</v>
+        <v>-3.604468882237792</v>
       </c>
       <c r="G7" t="n">
-        <v>126.1880406361023</v>
+        <v>125.9657787729132</v>
       </c>
       <c r="H7" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="8">
@@ -670,19 +670,19 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1.000579251593338</v>
+        <v>1.001278456154777</v>
       </c>
       <c r="E8" t="n">
-        <v>3911457565.724144</v>
+        <v>3938548447.226166</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0353966867897044</v>
+        <v>0.100939497354222</v>
       </c>
       <c r="G8" t="n">
-        <v>1.00145120391364</v>
+        <v>1.001476797453904</v>
       </c>
       <c r="H8" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="9">
@@ -700,19 +700,19 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1694094083317871</v>
+        <v>0.1703741125665958</v>
       </c>
       <c r="E9" t="n">
-        <v>587431862.6889677</v>
+        <v>594437659.180178</v>
       </c>
       <c r="F9" t="n">
-        <v>-6.583110759757824</v>
+        <v>-6.06862600745446</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1726923547804482</v>
+        <v>0.1722242722826475</v>
       </c>
       <c r="H9" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="10">
@@ -730,19 +730,19 @@
         <v>45000000000</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6719315847263519</v>
+        <v>0.6745334421358229</v>
       </c>
       <c r="E10" t="n">
-        <v>325216277.4983057</v>
+        <v>327578924.8543985</v>
       </c>
       <c r="F10" t="n">
-        <v>-5.18865294483043</v>
+        <v>-4.954127366025689</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6786383343146972</v>
+        <v>0.6776034453413297</v>
       </c>
       <c r="H10" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="11">
@@ -760,19 +760,19 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2304069582683168</v>
+        <v>0.2302783259612055</v>
       </c>
       <c r="E11" t="n">
-        <v>283548641.0543944</v>
+        <v>284280223.9630108</v>
       </c>
       <c r="F11" t="n">
-        <v>-1.061319468367403</v>
+        <v>-1.028240849361373</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2336074303263903</v>
+        <v>0.2334863945424018</v>
       </c>
       <c r="H11" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="12">
@@ -790,19 +790,19 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>1826.631634427173</v>
+        <v>1825.752863667699</v>
       </c>
       <c r="E12" t="n">
-        <v>6970701.536407065</v>
+        <v>6966864.279813101</v>
       </c>
       <c r="F12" t="n">
-        <v>-3.946098383456911</v>
+        <v>-4.03842628894656</v>
       </c>
       <c r="G12" t="n">
-        <v>1857.085591897561</v>
+        <v>1856.600704746712</v>
       </c>
       <c r="H12" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="13">
@@ -820,19 +820,19 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>82160.40858273028</v>
+        <v>82293.00008394162</v>
       </c>
       <c r="E13" t="n">
-        <v>112914807.3429569</v>
+        <v>113069494.8774586</v>
       </c>
       <c r="F13" t="n">
-        <v>-2.453226898889041</v>
+        <v>-2.363385773569916</v>
       </c>
       <c r="G13" t="n">
-        <v>82934.90814972202</v>
+        <v>82858.57567879203</v>
       </c>
       <c r="H13" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="14">
@@ -850,19 +850,19 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>3.655073712576874</v>
+        <v>3.670128622638756</v>
       </c>
       <c r="E14" t="n">
-        <v>89797936.8219194</v>
+        <v>90060417.19794378</v>
       </c>
       <c r="F14" t="n">
-        <v>-4.280354345389253</v>
+        <v>-3.833941653919497</v>
       </c>
       <c r="G14" t="n">
-        <v>3.7269633519303</v>
+        <v>3.718938445881623</v>
       </c>
       <c r="H14" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="15">
@@ -880,19 +880,19 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>13.49864936310586</v>
+        <v>13.55766616601435</v>
       </c>
       <c r="E15" t="n">
-        <v>148033444.5081975</v>
+        <v>149729896.9923917</v>
       </c>
       <c r="F15" t="n">
-        <v>-5.574427935687719</v>
+        <v>-5.105524365812474</v>
       </c>
       <c r="G15" t="n">
-        <v>13.77942534745326</v>
+        <v>13.74571805319632</v>
       </c>
       <c r="H15" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="16">
@@ -910,19 +910,19 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>9.581990713056573</v>
+        <v>9.592517627144282</v>
       </c>
       <c r="E16" t="n">
-        <v>5065218.850671666</v>
+        <v>5077252.470146463</v>
       </c>
       <c r="F16" t="n">
-        <v>-1.504257005189039</v>
+        <v>-1.343885281440595</v>
       </c>
       <c r="G16" t="n">
-        <v>9.546560172174159</v>
+        <v>9.546136462148755</v>
       </c>
       <c r="H16" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="17">
@@ -940,19 +940,19 @@
         <v>50001806812</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2665675637621393</v>
+        <v>0.2675161271012842</v>
       </c>
       <c r="E17" t="n">
-        <v>64188286.38827319</v>
+        <v>64409490.96026874</v>
       </c>
       <c r="F17" t="n">
-        <v>-3.219199548340176</v>
+        <v>-2.910396109676125</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2679960011734401</v>
+        <v>0.2676030983765726</v>
       </c>
       <c r="H17" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="18">
@@ -970,19 +970,19 @@
         <v>715748719</v>
       </c>
       <c r="D18" t="n">
-        <v>19.55359459533226</v>
+        <v>19.68883789366965</v>
       </c>
       <c r="E18" t="n">
-        <v>129822586.3204629</v>
+        <v>131347962.3695596</v>
       </c>
       <c r="F18" t="n">
-        <v>-4.141941735598029</v>
+        <v>-3.544833516869298</v>
       </c>
       <c r="G18" t="n">
-        <v>19.97315368157841</v>
+        <v>19.93961769465554</v>
       </c>
       <c r="H18" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="19">
@@ -1000,19 +1000,19 @@
         <v>589552695333683</v>
       </c>
       <c r="D19" t="n">
-        <v>1.26499357219e-05</v>
+        <v>1.27072729629e-05</v>
       </c>
       <c r="E19" t="n">
-        <v>86169843.15545613</v>
+        <v>86865024.13982321</v>
       </c>
       <c r="F19" t="n">
-        <v>-4.991596333347339</v>
+        <v>-4.63866863341444</v>
       </c>
       <c r="G19" t="n">
-        <v>1.28018528277e-05</v>
+        <v>1.27713982102e-05</v>
       </c>
       <c r="H19" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="20">
@@ -1030,19 +1030,19 @@
         <v>10000000000</v>
       </c>
       <c r="D20" t="n">
-        <v>2.297000399762225</v>
+        <v>2.309062851846233</v>
       </c>
       <c r="E20" t="n">
-        <v>600903513.5160155</v>
+        <v>603811213.5792202</v>
       </c>
       <c r="F20" t="n">
-        <v>-8.632187238565791</v>
+        <v>-8.380111858009318</v>
       </c>
       <c r="G20" t="n">
-        <v>2.372312924769421</v>
+        <v>2.357228397357926</v>
       </c>
       <c r="H20" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="21">
@@ -1060,19 +1060,19 @@
         <v>50000000000</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1717106537448069</v>
+        <v>0.1727124461220426</v>
       </c>
       <c r="E21" t="n">
-        <v>128136656.5223964</v>
+        <v>129297238.4542243</v>
       </c>
       <c r="F21" t="n">
-        <v>-5.886969332377054</v>
+        <v>-5.543462823116546</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1728983354961282</v>
+        <v>0.1726025041526711</v>
       </c>
       <c r="H21" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="22">
@@ -1090,19 +1090,19 @@
         <v>84000000</v>
       </c>
       <c r="D22" t="n">
-        <v>85.33712506630566</v>
+        <v>85.61918210119242</v>
       </c>
       <c r="E22" t="n">
-        <v>202371499.2088674</v>
+        <v>203624267.8348365</v>
       </c>
       <c r="F22" t="n">
-        <v>-2.690864602872835</v>
+        <v>-2.357580805374779</v>
       </c>
       <c r="G22" t="n">
-        <v>86.02107560858659</v>
+        <v>85.94390786870935</v>
       </c>
       <c r="H22" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="23">
@@ -1120,19 +1120,19 @@
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>4.049090198676905</v>
+        <v>4.080725676701681</v>
       </c>
       <c r="E23" t="n">
-        <v>83390845.62582777</v>
+        <v>84990974.29550412</v>
       </c>
       <c r="F23" t="n">
-        <v>-5.405762037050458</v>
+        <v>-4.691757297221193</v>
       </c>
       <c r="G23" t="n">
-        <v>4.123498331093471</v>
+        <v>4.115912367480848</v>
       </c>
       <c r="H23" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="24">
@@ -1150,19 +1150,19 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>1822.142819474041</v>
+        <v>1820.303492719007</v>
       </c>
       <c r="E24" t="n">
-        <v>458907602.7908561</v>
+        <v>458398419.59471</v>
       </c>
       <c r="F24" t="n">
-        <v>-4.23435710821229</v>
+        <v>-4.510485099114457</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="25">
@@ -1180,19 +1180,19 @@
         <v>888888888</v>
       </c>
       <c r="D25" t="n">
-        <v>6.237462988846933</v>
+        <v>6.26213749549555</v>
       </c>
       <c r="E25" t="n">
-        <v>31569193.10418135</v>
+        <v>31935081.26858781</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.3261219874268728</v>
+        <v>0.2400808515054984</v>
       </c>
       <c r="G25" t="n">
-        <v>6.189777067193133</v>
+        <v>6.187826864389828</v>
       </c>
       <c r="H25" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="26">
@@ -1210,19 +1210,19 @@
         <v>21000000</v>
       </c>
       <c r="D26" t="n">
-        <v>302.1037252063375</v>
+        <v>303.4525906130893</v>
       </c>
       <c r="E26" t="n">
-        <v>50145991.22062479</v>
+        <v>50523838.68709208</v>
       </c>
       <c r="F26" t="n">
-        <v>-1.684581706020147</v>
+        <v>-1.534200966876454</v>
       </c>
       <c r="G26" t="n">
-        <v>305.0693074417908</v>
+        <v>304.850549621333</v>
       </c>
       <c r="H26" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="27">
@@ -1240,19 +1240,19 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>4.637274702918074</v>
+        <v>4.648244786514637</v>
       </c>
       <c r="E27" t="n">
-        <v>128162231.7914895</v>
+        <v>128223484.9942609</v>
       </c>
       <c r="F27" t="n">
-        <v>-4.099453677840117</v>
+        <v>-4.072911163628737</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="28">
@@ -1270,19 +1270,19 @@
         <v>100000000000</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7963881382335473</v>
+        <v>0.7981116800254935</v>
       </c>
       <c r="E28" t="n">
-        <v>94508756.30466755</v>
+        <v>94983084.91939208</v>
       </c>
       <c r="F28" t="n">
-        <v>-4.174852537859113</v>
+        <v>-4.053573362150864</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="29">
@@ -1300,19 +1300,19 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.9996348531409276</v>
+        <v>0.9998210050652018</v>
       </c>
       <c r="E29" t="n">
-        <v>77398585.98155102</v>
+        <v>76516309.83574586</v>
       </c>
       <c r="F29" t="n">
-        <v>0.013150413164148</v>
+        <v>0.0317284179221477</v>
       </c>
       <c r="G29" t="n">
-        <v>0.999348299039692</v>
+        <v>0.999378558561045</v>
       </c>
       <c r="H29" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="30">
@@ -1330,19 +1330,19 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>0.9996415360319072</v>
+        <v>0.9997036594883386</v>
       </c>
       <c r="E30" t="n">
-        <v>42157230.07586022</v>
+        <v>42153539.50577791</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0399017562113137</v>
+        <v>0.0325274575496051</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="31">
@@ -1360,19 +1360,19 @@
         <v>1000000000</v>
       </c>
       <c r="D31" t="n">
-        <v>12.7738171619033</v>
+        <v>12.87350087974377</v>
       </c>
       <c r="E31" t="n">
-        <v>20372639.52308211</v>
+        <v>20604134.13641572</v>
       </c>
       <c r="F31" t="n">
-        <v>-5.451758495824202</v>
+        <v>-4.614718057507005</v>
       </c>
       <c r="G31" t="n">
-        <v>12.88370296938075</v>
+        <v>12.85377755483446</v>
       </c>
       <c r="H31" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="32">
@@ -1390,19 +1390,19 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>216.6459310203402</v>
+        <v>216.5043471615185</v>
       </c>
       <c r="E32" t="n">
-        <v>29343423.26593633</v>
+        <v>29365008.47897424</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.1608927974195777</v>
+        <v>-0.2779796124097036</v>
       </c>
       <c r="G32" t="n">
-        <v>216.2504398956469</v>
+        <v>216.1808981338185</v>
       </c>
       <c r="H32" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="33">
@@ -1420,19 +1420,19 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>5.957023212775063</v>
+        <v>5.997394508584185</v>
       </c>
       <c r="E33" t="n">
-        <v>62308366.23531105</v>
+        <v>61876197.04852512</v>
       </c>
       <c r="F33" t="n">
-        <v>-4.115363033295562</v>
+        <v>-3.416881010198233</v>
       </c>
       <c r="G33" t="n">
-        <v>6.072844576788096</v>
+        <v>6.057285326028802</v>
       </c>
       <c r="H33" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="34">
@@ -1450,19 +1450,19 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>5.206102070472038</v>
+        <v>5.223393202934701</v>
       </c>
       <c r="E34" t="n">
-        <v>49178999.82395692</v>
+        <v>49438667.37895875</v>
       </c>
       <c r="F34" t="n">
-        <v>-6.463045583427394</v>
+        <v>-6.299126473365803</v>
       </c>
       <c r="G34" t="n">
-        <v>5.357840078210184</v>
+        <v>5.34913778345696</v>
       </c>
       <c r="H34" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="35">
@@ -1480,19 +1480,19 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>2.56616655832448</v>
+        <v>2.584789059970015</v>
       </c>
       <c r="E35" t="n">
-        <v>73565751.96209612</v>
+        <v>74241312.14129223</v>
       </c>
       <c r="F35" t="n">
-        <v>-6.173148362971326</v>
+        <v>-5.57141819633397</v>
       </c>
       <c r="G35" t="n">
-        <v>2.63624076837057</v>
+        <v>2.631273174115652</v>
       </c>
       <c r="H35" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="36">
@@ -1510,19 +1510,19 @@
         <v>420690000000000</v>
       </c>
       <c r="D36" t="n">
-        <v>7.1694614843e-06</v>
+        <v>7.2019165067e-06</v>
       </c>
       <c r="E36" t="n">
-        <v>322405478.4250872</v>
+        <v>324447816.0335299</v>
       </c>
       <c r="F36" t="n">
-        <v>-8.5531366898791</v>
+        <v>-8.178375055183244</v>
       </c>
       <c r="G36" t="n">
-        <v>7.4507509335e-06</v>
+        <v>7.4251425768e-06</v>
       </c>
       <c r="H36" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="37">
@@ -1540,19 +1540,19 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>48.18430711928305</v>
+        <v>48.19366959066517</v>
       </c>
       <c r="E37" t="n">
-        <v>2152628.768638705</v>
+        <v>2172852.576908858</v>
       </c>
       <c r="F37" t="n">
-        <v>-2.018904381926386</v>
+        <v>-2.030974933212208</v>
       </c>
       <c r="G37" t="n">
-        <v>48.64497113544613</v>
+        <v>48.22096277802032</v>
       </c>
       <c r="H37" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="38">
@@ -1570,19 +1570,19 @@
         <v>30263013692</v>
       </c>
       <c r="D38" t="n">
-        <v>0.1039377989195878</v>
+        <v>0.1050054112391722</v>
       </c>
       <c r="E38" t="n">
-        <v>30687296.77431269</v>
+        <v>31308438.81772804</v>
       </c>
       <c r="F38" t="n">
-        <v>2.948178007482119</v>
+        <v>4.407271675063641</v>
       </c>
       <c r="G38" t="n">
-        <v>0.1009154167014576</v>
+        <v>0.1014797713652044</v>
       </c>
       <c r="H38" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="39">
@@ -1600,19 +1600,19 @@
         <v>6219316795</v>
       </c>
       <c r="D39" t="n">
-        <v>0.8003969388846803</v>
+        <v>0.80243885417295</v>
       </c>
       <c r="E39" t="n">
-        <v>89110784.78888534</v>
+        <v>89062690.90208563</v>
       </c>
       <c r="F39" t="n">
-        <v>-4.013899707555161</v>
+        <v>-3.878696371064016</v>
       </c>
       <c r="G39" t="n">
-        <v>0.8141420282944772</v>
+        <v>0.812877100848315</v>
       </c>
       <c r="H39" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="40">
@@ -1630,19 +1630,19 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.9985393929047</v>
+        <v>0.9984440841840216</v>
       </c>
       <c r="E40" t="n">
-        <v>1575702421.302977</v>
+        <v>1580817680.88182</v>
       </c>
       <c r="F40" t="n">
-        <v>-0.0801736221960067</v>
+        <v>-0.0794863613942713</v>
       </c>
       <c r="G40" t="n">
-        <v>0.9986698156804152</v>
+        <v>0.998667843755949</v>
       </c>
       <c r="H40" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="41">
@@ -1660,19 +1660,19 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>5.341970798224012</v>
+        <v>5.355358167420772</v>
       </c>
       <c r="E41" t="n">
-        <v>30048534.16580131</v>
+        <v>30285562.28965387</v>
       </c>
       <c r="F41" t="n">
-        <v>-5.041677432508983</v>
+        <v>-4.777911829324881</v>
       </c>
       <c r="G41" t="n">
-        <v>5.416678375289444</v>
+        <v>5.402828778999718</v>
       </c>
       <c r="H41" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="42">
@@ -1690,19 +1690,19 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>167.4715235081837</v>
+        <v>168.9382108748585</v>
       </c>
       <c r="E42" t="n">
-        <v>130492580.9391714</v>
+        <v>132152343.37039</v>
       </c>
       <c r="F42" t="n">
-        <v>-4.895071614169458</v>
+        <v>-3.975614576502062</v>
       </c>
       <c r="G42" t="n">
-        <v>173.8869159622273</v>
+        <v>173.3192129933889</v>
       </c>
       <c r="H42" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="43">
@@ -1720,19 +1720,19 @@
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>0.7960019162448302</v>
+        <v>0.8014353330087522</v>
       </c>
       <c r="E43" t="n">
-        <v>120968245.5405302</v>
+        <v>121732495.5327971</v>
       </c>
       <c r="F43" t="n">
-        <v>-6.057005787335703</v>
+        <v>-5.438096251317057</v>
       </c>
       <c r="G43" t="n">
-        <v>0.8043753579066322</v>
+        <v>0.802986251555848</v>
       </c>
       <c r="H43" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="44">
@@ -1750,19 +1750,19 @@
         <v>210700000</v>
       </c>
       <c r="D44" t="n">
-        <v>16.56381550975512</v>
+        <v>16.63265775452665</v>
       </c>
       <c r="E44" t="n">
-        <v>24803475.43751689</v>
+        <v>24964659.99460781</v>
       </c>
       <c r="F44" t="n">
-        <v>-3.486286738575677</v>
+        <v>-3.042675613588077</v>
       </c>
       <c r="G44" t="n">
-        <v>16.81358544575735</v>
+        <v>16.79478605105006</v>
       </c>
       <c r="H44" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="45">
@@ -1780,19 +1780,19 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.2022508779883776</v>
+        <v>0.2029858218806858</v>
       </c>
       <c r="E45" t="n">
-        <v>41272510.16574624</v>
+        <v>41496019.78333586</v>
       </c>
       <c r="F45" t="n">
-        <v>-4.946455860364696</v>
+        <v>-4.535668225778547</v>
       </c>
       <c r="G45" t="n">
-        <v>0.2040717464484717</v>
+        <v>0.2036532869851435</v>
       </c>
       <c r="H45" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="46">
@@ -1810,19 +1810,19 @@
         <v>999999993.45</v>
       </c>
       <c r="D46" t="n">
-        <v>10.03814972102562</v>
+        <v>10.08969062238289</v>
       </c>
       <c r="E46" t="n">
-        <v>88676169.63886042</v>
+        <v>89731895.7149255</v>
       </c>
       <c r="F46" t="n">
-        <v>-3.50348009159051</v>
+        <v>-3.351595464050587</v>
       </c>
       <c r="G46" t="n">
-        <v>10.12015917940824</v>
+        <v>10.10803013645091</v>
       </c>
       <c r="H46" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="47">
@@ -1840,19 +1840,19 @@
         <v>86712634466</v>
       </c>
       <c r="D47" t="n">
-        <v>0.0227834610011582</v>
+        <v>0.0229385489581322</v>
       </c>
       <c r="E47" t="n">
-        <v>22757160.47829301</v>
+        <v>23020385.90441527</v>
       </c>
       <c r="F47" t="n">
-        <v>-5.479480736354565</v>
+        <v>-4.935783029477224</v>
       </c>
       <c r="G47" t="n">
-        <v>0.0231585935657915</v>
+        <v>0.0231168750144423</v>
       </c>
       <c r="H47" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="48">
@@ -1870,19 +1870,19 @@
         <v>21000000</v>
       </c>
       <c r="D48" t="n">
-        <v>229.2026689030462</v>
+        <v>230.7049429611233</v>
       </c>
       <c r="E48" t="n">
-        <v>69504153.98012163</v>
+        <v>69873874.3706418</v>
       </c>
       <c r="F48" t="n">
-        <v>-5.840516107542122</v>
+        <v>-5.472488288918324</v>
       </c>
       <c r="G48" t="n">
-        <v>230.2406184801843</v>
+        <v>229.9681160090976</v>
       </c>
       <c r="H48" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="49">
@@ -1900,19 +1900,19 @@
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.3634299649769541</v>
+        <v>0.3654066609858666</v>
       </c>
       <c r="E49" t="n">
-        <v>85826748.80291852</v>
+        <v>86603642.78837593</v>
       </c>
       <c r="F49" t="n">
-        <v>-6.152872201687339</v>
+        <v>-5.840256217823335</v>
       </c>
       <c r="G49" t="n">
-        <v>0.3761115254978733</v>
+        <v>0.3755070902972269</v>
       </c>
       <c r="H49" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="50">
@@ -1930,19 +1930,19 @@
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>22.24514005752849</v>
+        <v>22.30136333714398</v>
       </c>
       <c r="E50" t="n">
-        <v>8371357.368065163</v>
+        <v>8402986.17092145</v>
       </c>
       <c r="F50" t="n">
-        <v>-2.973644472234199</v>
+        <v>-2.653674354782696</v>
       </c>
       <c r="G50" t="n">
-        <v>22.49397454147745</v>
+        <v>22.46080518153678</v>
       </c>
       <c r="H50" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="51">
@@ -1960,19 +1960,19 @@
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>3.200773351343412</v>
+        <v>3.212281851458217</v>
       </c>
       <c r="E51" t="n">
-        <v>32420868.58766641</v>
+        <v>32496108.21636644</v>
       </c>
       <c r="F51" t="n">
-        <v>-6.707107306547996</v>
+        <v>-6.508465078754236</v>
       </c>
       <c r="G51" t="n">
-        <v>3.28469445686484</v>
+        <v>3.273771767168606</v>
       </c>
       <c r="H51" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="52">
@@ -1990,19 +1990,19 @@
         <v>644168762</v>
       </c>
       <c r="D52" t="n">
-        <v>3.461186761949088</v>
+        <v>3.480388051229566</v>
       </c>
       <c r="E52" t="n">
-        <v>43895960.4035756</v>
+        <v>44847856.33745009</v>
       </c>
       <c r="F52" t="n">
-        <v>-7.889060486973999</v>
+        <v>-7.678750092370467</v>
       </c>
       <c r="G52" t="n">
-        <v>3.618771257966712</v>
+        <v>3.596944400112978</v>
       </c>
       <c r="H52" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="53">
@@ -2020,19 +2020,19 @@
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>2.723158295605205</v>
+        <v>2.735973682964012</v>
       </c>
       <c r="E53" t="n">
-        <v>60728871.61596602</v>
+        <v>60914112.01474593</v>
       </c>
       <c r="F53" t="n">
-        <v>-4.01899654682012</v>
+        <v>-3.585678841324242</v>
       </c>
       <c r="G53" t="n">
-        <v>2.779118139968536</v>
+        <v>2.774611319132584</v>
       </c>
       <c r="H53" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="54">
@@ -2050,19 +2050,19 @@
         <v>28704026601</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0641139039405092</v>
+        <v>0.0642964576819243</v>
       </c>
       <c r="E54" t="n">
-        <v>45114767.62453119</v>
+        <v>45257356.04440505</v>
       </c>
       <c r="F54" t="n">
-        <v>-8.168709503473734</v>
+        <v>-8.014852462378961</v>
       </c>
       <c r="G54" t="n">
-        <v>0.06501335342196859</v>
+        <v>0.0649115868391312</v>
       </c>
       <c r="H54" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="55">
@@ -2080,19 +2080,19 @@
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>4.208947650175097</v>
+        <v>4.232697784274436</v>
       </c>
       <c r="E55" t="n">
-        <v>54137335.75386728</v>
+        <v>54558054.13450658</v>
       </c>
       <c r="F55" t="n">
-        <v>-7.30815804212294</v>
+        <v>-6.716694956653594</v>
       </c>
       <c r="G55" t="n">
-        <v>4.385814131030191</v>
+        <v>4.375891895877328</v>
       </c>
       <c r="H55" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="56">
@@ -2110,19 +2110,19 @@
         <v>10000000000</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1833873675677493</v>
+        <v>0.1843582935250483</v>
       </c>
       <c r="E56" t="n">
-        <v>44625472.41009375</v>
+        <v>44950777.34959612</v>
       </c>
       <c r="F56" t="n">
-        <v>-8.045959901924652</v>
+        <v>-7.522938270177661</v>
       </c>
       <c r="G56" t="n">
-        <v>0.1882228009118393</v>
+        <v>0.1877839629998194</v>
       </c>
       <c r="H56" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="57">
@@ -2140,19 +2140,19 @@
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>0.3317757903515358</v>
+        <v>0.3337681418140623</v>
       </c>
       <c r="E57" t="n">
-        <v>72256852.93873942</v>
+        <v>73495471.42484793</v>
       </c>
       <c r="F57" t="n">
-        <v>-4.694962803552409</v>
+        <v>-4.089026656567444</v>
       </c>
       <c r="G57" t="n">
-        <v>0.3347457808490293</v>
+        <v>0.3342787286153585</v>
       </c>
       <c r="H57" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="58">
@@ -2170,19 +2170,19 @@
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>17.56778844236263</v>
+        <v>17.52388946628782</v>
       </c>
       <c r="E58" t="n">
-        <v>13220717.83450496</v>
+        <v>12408498.79721028</v>
       </c>
       <c r="F58" t="n">
-        <v>-4.671229924768629</v>
+        <v>-4.910961552126381</v>
       </c>
       <c r="G58" t="n">
-        <v>18.0306465294782</v>
+        <v>18.0010427894502</v>
       </c>
       <c r="H58" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="59">
@@ -2200,19 +2200,19 @@
         <v>3175000000</v>
       </c>
       <c r="D59" t="n">
-        <v>0.4849823297451328</v>
+        <v>0.4898708196738049</v>
       </c>
       <c r="E59" t="n">
-        <v>93429676.35674819</v>
+        <v>94586902.37159176</v>
       </c>
       <c r="F59" t="n">
-        <v>-10.50882598656552</v>
+        <v>-9.475287569623987</v>
       </c>
       <c r="G59" t="n">
-        <v>0.5028413180145808</v>
+        <v>0.5009069681711168</v>
       </c>
       <c r="H59" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="60">
@@ -2230,19 +2230,19 @@
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>5.239154985647333</v>
+        <v>5.29543645381861</v>
       </c>
       <c r="E60" t="n">
-        <v>34248273.13398734</v>
+        <v>34551655.5949595</v>
       </c>
       <c r="F60" t="n">
-        <v>-3.937378280250306</v>
+        <v>-3.290323686465688</v>
       </c>
       <c r="G60" t="n">
-        <v>5.304690468160249</v>
+        <v>5.293664393258978</v>
       </c>
       <c r="H60" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="61">
@@ -2260,19 +2260,19 @@
         <v>200000000</v>
       </c>
       <c r="D61" t="n">
-        <v>11.05155376106706</v>
+        <v>11.07150030176666</v>
       </c>
       <c r="E61" t="n">
-        <v>638155.6177684378</v>
+        <v>641288.7701626321</v>
       </c>
       <c r="F61" t="n">
-        <v>-0.964817857730126</v>
+        <v>-0.8619525572045404</v>
       </c>
       <c r="G61" t="n">
-        <v>11.07794738852414</v>
+        <v>11.07424464591755</v>
       </c>
       <c r="H61" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="62">
@@ -2290,19 +2290,19 @@
         <v>3000000000</v>
       </c>
       <c r="D62" t="n">
-        <v>0.4744200940296352</v>
+        <v>0.4771304541329743</v>
       </c>
       <c r="E62" t="n">
-        <v>25887501.63028597</v>
+        <v>26160665.64849852</v>
       </c>
       <c r="F62" t="n">
-        <v>-4.8879280183415</v>
+        <v>-4.431489448361488</v>
       </c>
       <c r="G62" t="n">
-        <v>0.4723689064591215</v>
+        <v>0.471647679797115</v>
       </c>
       <c r="H62" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="63">
@@ -2320,19 +2320,19 @@
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>0.7643105408630777</v>
+        <v>0.7692184030064616</v>
       </c>
       <c r="E63" t="n">
-        <v>56353053.5764173</v>
+        <v>57286716.03179077</v>
       </c>
       <c r="F63" t="n">
-        <v>-8.455617740187167</v>
+        <v>-7.96111694338625</v>
       </c>
       <c r="G63" t="n">
-        <v>0.7867260737979288</v>
+        <v>0.7850005165233475</v>
       </c>
       <c r="H63" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="64">
@@ -2350,19 +2350,19 @@
         <v>2630547141</v>
       </c>
       <c r="D64" t="n">
-        <v>0.4696050579380655</v>
+        <v>0.472712210363298</v>
       </c>
       <c r="E64" t="n">
-        <v>54920270.07027698</v>
+        <v>55509764.42245329</v>
       </c>
       <c r="F64" t="n">
-        <v>-7.721933664580022</v>
+        <v>-7.216216619898908</v>
       </c>
       <c r="G64" t="n">
-        <v>0.4831587145785492</v>
+        <v>0.4819306928483113</v>
       </c>
       <c r="H64" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="65">
@@ -2380,19 +2380,19 @@
         <v>10000000000</v>
       </c>
       <c r="D65" t="n">
-        <v>0.4448802175468912</v>
+        <v>0.448974683147663</v>
       </c>
       <c r="E65" t="n">
-        <v>76197939.52469747</v>
+        <v>77037706.20009713</v>
       </c>
       <c r="F65" t="n">
-        <v>-7.899119197540935</v>
+        <v>-7.22043603089161</v>
       </c>
       <c r="G65" t="n">
-        <v>0.4746995954653084</v>
+        <v>0.4732417511268104</v>
       </c>
       <c r="H65" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="66">
@@ -2410,19 +2410,19 @@
         <v>1000000</v>
       </c>
       <c r="D66" t="n">
-        <v>1283.855512648185</v>
+        <v>1293.693815483873</v>
       </c>
       <c r="E66" t="n">
-        <v>38937342.10592522</v>
+        <v>38646153.48055481</v>
       </c>
       <c r="F66" t="n">
-        <v>-11.81798731418845</v>
+        <v>-11.11440358369486</v>
       </c>
       <c r="G66" t="n">
-        <v>1377.378779244615</v>
+        <v>1365.665191743982</v>
       </c>
       <c r="H66" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="67">
@@ -2440,19 +2440,19 @@
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>0.0681997463540025</v>
+        <v>0.0681947718721061</v>
       </c>
       <c r="E67" t="n">
-        <v>8142955.267243866</v>
+        <v>8141779.505972645</v>
       </c>
       <c r="F67" t="n">
-        <v>-2.091941948004824</v>
+        <v>-2.065145784434361</v>
       </c>
       <c r="G67" t="n">
-        <v>0.06880218916029721</v>
+        <v>0.0687431017553435</v>
       </c>
       <c r="H67" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="68">
@@ -2470,19 +2470,19 @@
         <v>2000000000</v>
       </c>
       <c r="D68" t="n">
-        <v>0.5485133137658671</v>
+        <v>0.5521243630488309</v>
       </c>
       <c r="E68" t="n">
-        <v>10262888.14573162</v>
+        <v>10365674.7558606</v>
       </c>
       <c r="F68" t="n">
-        <v>-5.524921352215078</v>
+        <v>-5.189069564354593</v>
       </c>
       <c r="G68" t="n">
-        <v>0.5622747964606907</v>
+        <v>0.5607393093750623</v>
       </c>
       <c r="H68" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="69">
@@ -2500,19 +2500,19 @@
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>603.8202917871117</v>
+        <v>607.697966198818</v>
       </c>
       <c r="E69" t="n">
-        <v>11301114.45773778</v>
+        <v>11373689.10114176</v>
       </c>
       <c r="F69" t="n">
-        <v>-3.181186364492896</v>
+        <v>-2.820048211355692</v>
       </c>
       <c r="G69" t="n">
         <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="70">
@@ -2530,19 +2530,19 @@
         <v>1818000000</v>
       </c>
       <c r="D70" t="n">
-        <v>0.6223506842340983</v>
+        <v>0.6265865247348464</v>
       </c>
       <c r="E70" t="n">
-        <v>18885875.94140019</v>
+        <v>19027774.49477397</v>
       </c>
       <c r="F70" t="n">
-        <v>-5.664908629475115</v>
+        <v>-4.945153182347511</v>
       </c>
       <c r="G70" t="n">
-        <v>0.6292294061095763</v>
+        <v>0.6265622914257434</v>
       </c>
       <c r="H70" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="71">
@@ -2560,19 +2560,19 @@
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>0.7739677945459865</v>
+        <v>0.7788064684079382</v>
       </c>
       <c r="E71" t="n">
-        <v>72317537.6205415</v>
+        <v>72832124.25389594</v>
       </c>
       <c r="F71" t="n">
-        <v>-8.304888582817776</v>
+        <v>-7.730328906856132</v>
       </c>
       <c r="G71" t="n">
-        <v>0.8001925716231685</v>
+        <v>0.7984820503301564</v>
       </c>
       <c r="H71" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="72">
@@ -2590,19 +2590,19 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>0.9976964783104504</v>
+        <v>0.9976964985523024</v>
       </c>
       <c r="E72" t="n">
-        <v>22221876.25546323</v>
+        <v>22220725.70046323</v>
       </c>
       <c r="F72" t="n">
-        <v>0.0011156652422023</v>
+        <v>-0.002284651077521</v>
       </c>
       <c r="G72" t="n">
         <v>0</v>
       </c>
       <c r="H72" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="73">
@@ -2620,19 +2620,19 @@
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>1.12892594854e-05</v>
+        <v>1.13640330586e-05</v>
       </c>
       <c r="E73" t="n">
-        <v>53492670.76428469</v>
+        <v>53794434.80229677</v>
       </c>
       <c r="F73" t="n">
-        <v>-8.363662383718895</v>
+        <v>-7.858075964310598</v>
       </c>
       <c r="G73" t="n">
-        <v>1.15616252007e-05</v>
+        <v>1.15118747924e-05</v>
       </c>
       <c r="H73" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="74">
@@ -2650,19 +2650,19 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>0.1797293094238838</v>
+        <v>0.1807302139807161</v>
       </c>
       <c r="E74" t="n">
-        <v>48230289.15947066</v>
+        <v>48755190.3846544</v>
       </c>
       <c r="F74" t="n">
-        <v>-6.451273726046038</v>
+        <v>-6.015983318734015</v>
       </c>
       <c r="G74" t="n">
-        <v>0.1821464847958657</v>
+        <v>0.1817410755645439</v>
       </c>
       <c r="H74" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="75">
@@ -2680,19 +2680,19 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>0.0886614482151354</v>
+        <v>0.0893984898375097</v>
       </c>
       <c r="E75" t="n">
-        <v>10742740.43325384</v>
+        <v>10822210.61181171</v>
       </c>
       <c r="F75" t="n">
-        <v>-6.874338748587629</v>
+        <v>-6.018116139362933</v>
       </c>
       <c r="G75" t="n">
-        <v>0.0913646475318233</v>
+        <v>0.09110736386917929</v>
       </c>
       <c r="H75" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="76">
@@ -2710,19 +2710,19 @@
         <v>100000000</v>
       </c>
       <c r="D76" t="n">
-        <v>8.727175848469148</v>
+        <v>8.77383560231317</v>
       </c>
       <c r="E76" t="n">
-        <v>45775295.80938108</v>
+        <v>46150998.90039462</v>
       </c>
       <c r="F76" t="n">
-        <v>-5.622927175884642</v>
+        <v>-4.956532422652955</v>
       </c>
       <c r="G76" t="n">
-        <v>8.91105329911961</v>
+        <v>8.873629055578359</v>
       </c>
       <c r="H76" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="77">
@@ -2740,19 +2740,19 @@
         <v>2100000000</v>
       </c>
       <c r="D77" t="n">
-        <v>0.5441020272576751</v>
+        <v>0.5474245526509444</v>
       </c>
       <c r="E77" t="n">
-        <v>59388903.70260775</v>
+        <v>59410841.55956086</v>
       </c>
       <c r="F77" t="n">
-        <v>-4.179906125569557</v>
+        <v>-3.722061381327582</v>
       </c>
       <c r="G77" t="n">
-        <v>0.561913517779402</v>
+        <v>0.5606892622302188</v>
       </c>
       <c r="H77" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="78">
@@ -2770,19 +2770,19 @@
         <v>14881364</v>
       </c>
       <c r="D78" t="n">
-        <v>69.37486474912872</v>
+        <v>69.64116766977109</v>
       </c>
       <c r="E78" t="n">
-        <v>10675463.9206837</v>
+        <v>10711992.15846364</v>
       </c>
       <c r="F78" t="n">
-        <v>-3.134731057667506</v>
+        <v>-2.717335748385156</v>
       </c>
       <c r="G78" t="n">
-        <v>69.37812644007207</v>
+        <v>69.28114016879941</v>
       </c>
       <c r="H78" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="79">
@@ -2800,19 +2800,19 @@
         <v>1000000000</v>
       </c>
       <c r="D79" t="n">
-        <v>0.8307004320442866</v>
+        <v>0.8360399723196338</v>
       </c>
       <c r="E79" t="n">
-        <v>9397271.335065609</v>
+        <v>9499187.305290477</v>
       </c>
       <c r="F79" t="n">
-        <v>-6.838924235659997</v>
+        <v>-6.193998374036033</v>
       </c>
       <c r="G79" t="n">
-        <v>0.8517306820074946</v>
+        <v>0.8496616412330231</v>
       </c>
       <c r="H79" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="80">
@@ -2830,19 +2830,19 @@
         <v>580000000</v>
       </c>
       <c r="D80" t="n">
-        <v>2.162633544985372</v>
+        <v>2.174049400562978</v>
       </c>
       <c r="E80" t="n">
-        <v>3994703.773199595</v>
+        <v>4020821.143730174</v>
       </c>
       <c r="F80" t="n">
-        <v>-4.249042400581502</v>
+        <v>-4.243700945416238</v>
       </c>
       <c r="G80" t="n">
         <v>0</v>
       </c>
       <c r="H80" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="81">
@@ -2860,19 +2860,19 @@
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>0.0132099956544099</v>
+        <v>0.0132326225574872</v>
       </c>
       <c r="E81" t="n">
-        <v>11999002.61338104</v>
+        <v>12040100.98384464</v>
       </c>
       <c r="F81" t="n">
-        <v>-3.876904907918119</v>
+        <v>-3.688709851325987</v>
       </c>
       <c r="G81" t="n">
-        <v>0.0133742920755036</v>
+        <v>0.0133463487595621</v>
       </c>
       <c r="H81" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="82">
@@ -2890,19 +2890,19 @@
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>0.9982620237116672</v>
+        <v>0.9983127064537924</v>
       </c>
       <c r="E82" t="n">
-        <v>8939006.081061056</v>
+        <v>8947105.451813435</v>
       </c>
       <c r="F82" t="n">
-        <v>-0.1806435559488069</v>
+        <v>-0.1815774802922565</v>
       </c>
       <c r="G82" t="n">
-        <v>0.9985215089226388</v>
+        <v>0.9984617540967416</v>
       </c>
       <c r="H82" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="83">
@@ -2920,19 +2920,19 @@
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>7.361434811137042</v>
+        <v>7.397914870883448</v>
       </c>
       <c r="E83" t="n">
-        <v>148966341.3839508</v>
+        <v>147650655.9995573</v>
       </c>
       <c r="F83" t="n">
-        <v>-16.66330032111655</v>
+        <v>-16.42561681298717</v>
       </c>
       <c r="G83" t="n">
-        <v>8.086417063358727</v>
+        <v>8.015196342727146</v>
       </c>
       <c r="H83" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="84">
@@ -2950,19 +2950,19 @@
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>0.870330002256832</v>
+        <v>0.8781661326532031</v>
       </c>
       <c r="E84" t="n">
-        <v>39392005.75798941</v>
+        <v>39861790.59051279</v>
       </c>
       <c r="F84" t="n">
-        <v>-7.123272956097913</v>
+        <v>-6.443070896768138</v>
       </c>
       <c r="G84" t="n">
-        <v>0.904567314271282</v>
+        <v>0.9024296962588342</v>
       </c>
       <c r="H84" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="85">
@@ -2980,19 +2980,19 @@
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>3113.88773060434</v>
+        <v>3113.811825636049</v>
       </c>
       <c r="E85" t="n">
-        <v>6505929.295504448</v>
+        <v>6521254.651175963</v>
       </c>
       <c r="F85" t="n">
-        <v>0.2324938147597639</v>
+        <v>0.240516074570105</v>
       </c>
       <c r="G85" t="n">
-        <v>3111.819718044713</v>
+        <v>3111.97268421377</v>
       </c>
       <c r="H85" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="86">
@@ -3010,19 +3010,19 @@
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>1.075929622988704</v>
+        <v>1.078356661010723</v>
       </c>
       <c r="E86" t="n">
-        <v>3344034.538967133</v>
+        <v>3354281.476515043</v>
       </c>
       <c r="F86" t="n">
-        <v>-3.872798978640378</v>
+        <v>-3.669043980278602</v>
       </c>
       <c r="G86" t="n">
-        <v>1.088314174680323</v>
+        <v>1.087284605181189</v>
       </c>
       <c r="H86" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="87">
@@ -3040,79 +3040,79 @@
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>2.194707106111947</v>
+        <v>2.206260012016696</v>
       </c>
       <c r="E87" t="n">
-        <v>13341133.95427528</v>
+        <v>13501738.88255338</v>
       </c>
       <c r="F87" t="n">
-        <v>-1.57496694221837</v>
+        <v>-1.05725926064315</v>
       </c>
       <c r="G87" t="n">
-        <v>2.16526308256968</v>
+        <v>2.16381071840535</v>
       </c>
       <c r="H87" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>tezos</t>
+          <t>gala</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>XTZ</t>
+          <t>GALA</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>50000000000</v>
       </c>
       <c r="D88" t="n">
-        <v>0.6491911161441259</v>
+        <v>0.0154519859083297</v>
       </c>
       <c r="E88" t="n">
-        <v>9733887.588373197</v>
+        <v>38670584.455144</v>
       </c>
       <c r="F88" t="n">
-        <v>-4.185247168088681</v>
+        <v>-7.244844529664358</v>
       </c>
       <c r="G88" t="n">
-        <v>0.6637110068922031</v>
+        <v>0.0155755438700855</v>
       </c>
       <c r="H88" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>gala</t>
+          <t>tezos</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>GALA</t>
+          <t>XTZ</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>50000000000</v>
+        <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>0.0153273036288905</v>
+        <v>0.6498973145992833</v>
       </c>
       <c r="E89" t="n">
-        <v>38156480.37939525</v>
+        <v>9784674.578189235</v>
       </c>
       <c r="F89" t="n">
-        <v>-7.866606281884973</v>
+        <v>-4.083726145111177</v>
       </c>
       <c r="G89" t="n">
-        <v>0.0156240585593196</v>
+        <v>0.6629573109917954</v>
       </c>
       <c r="H89" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="90">
@@ -3130,19 +3130,19 @@
         <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>0.2690171720934153</v>
+        <v>0.27001769406763</v>
       </c>
       <c r="E90" t="n">
-        <v>15313112.44455382</v>
+        <v>15437541.00032419</v>
       </c>
       <c r="F90" t="n">
-        <v>-4.050687742001519</v>
+        <v>-3.694955399782808</v>
       </c>
       <c r="G90" t="n">
-        <v>0.2726459687979406</v>
+        <v>0.2719935528067818</v>
       </c>
       <c r="H90" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="91">
@@ -3160,19 +3160,19 @@
         <v>0</v>
       </c>
       <c r="D91" t="n">
-        <v>6.725345523e-07</v>
+        <v>6.726925356e-07</v>
       </c>
       <c r="E91" t="n">
-        <v>1117956.492391713</v>
+        <v>1119582.55069419</v>
       </c>
       <c r="F91" t="n">
-        <v>-1.036917634831299</v>
+        <v>-1.144621068620583</v>
       </c>
       <c r="G91" t="n">
-        <v>6.787313542e-07</v>
+        <v>6.785067114e-07</v>
       </c>
       <c r="H91" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="92">
@@ -3190,19 +3190,19 @@
         <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>3118.439354974003</v>
+        <v>3120.391715511204</v>
       </c>
       <c r="E92" t="n">
-        <v>46961060.14689401</v>
+        <v>47179474.36029996</v>
       </c>
       <c r="F92" t="n">
-        <v>0.7794311876670654</v>
+        <v>0.8938231713416683</v>
       </c>
       <c r="G92" t="n">
-        <v>3104.106441602849</v>
+        <v>3106.213260630469</v>
       </c>
       <c r="H92" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="93">
@@ -3220,19 +3220,19 @@
         <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>0.1729546685498464</v>
+        <v>0.1744014464748732</v>
       </c>
       <c r="E93" t="n">
-        <v>10752417.7391427</v>
+        <v>11074007.92505747</v>
       </c>
       <c r="F93" t="n">
-        <v>-5.878607012422229</v>
+        <v>-5.04205547579715</v>
       </c>
       <c r="G93" t="n">
-        <v>0.1753388064911254</v>
+        <v>0.1749882961790816</v>
       </c>
       <c r="H93" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="94">
@@ -3250,19 +3250,19 @@
         <v>3030303030.299</v>
       </c>
       <c r="D94" t="n">
-        <v>0.4874479490292167</v>
+        <v>0.4917164978778142</v>
       </c>
       <c r="E94" t="n">
-        <v>43863980.49589213</v>
+        <v>44371785.7632005</v>
       </c>
       <c r="F94" t="n">
-        <v>-4.786932064731952</v>
+        <v>-4.328137202239909</v>
       </c>
       <c r="G94" t="n">
-        <v>0.4891359202111243</v>
+        <v>0.4883480961803173</v>
       </c>
       <c r="H94" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="95">
@@ -3280,19 +3280,19 @@
         <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>31.12844986236473</v>
+        <v>31.16992377200446</v>
       </c>
       <c r="E95" t="n">
-        <v>8021229.032922717</v>
+        <v>8035242.495236797</v>
       </c>
       <c r="F95" t="n">
-        <v>-5.508927697391403</v>
+        <v>-5.36077167890005</v>
       </c>
       <c r="G95" t="n">
-        <v>32.16802660697675</v>
+        <v>32.11343468342404</v>
       </c>
       <c r="H95" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="96">
@@ -3310,19 +3310,19 @@
         <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>0.1022988982820189</v>
+        <v>0.1025970098339907</v>
       </c>
       <c r="E96" t="n">
-        <v>5943755.803454272</v>
+        <v>5963499.473332029</v>
       </c>
       <c r="F96" t="n">
-        <v>-3.83614497594405</v>
+        <v>-3.502170642702663</v>
       </c>
       <c r="G96" t="n">
-        <v>0.1035489193639471</v>
+        <v>0.1034965879236058</v>
       </c>
       <c r="H96" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="97">
@@ -3340,19 +3340,19 @@
         <v>450000000</v>
       </c>
       <c r="D97" t="n">
-        <v>1.988481670811483</v>
+        <v>2.000466894716783</v>
       </c>
       <c r="E97" t="n">
-        <v>60071163.68201321</v>
+        <v>60670783.59475005</v>
       </c>
       <c r="F97" t="n">
-        <v>-7.318169470205025</v>
+        <v>-6.464626824762689</v>
       </c>
       <c r="G97" t="n">
-        <v>2.012541646846876</v>
+        <v>2.008554710448774</v>
       </c>
       <c r="H97" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="98">
@@ -3370,19 +3370,19 @@
         <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>0.3769956106414815</v>
+        <v>0.3778741654980206</v>
       </c>
       <c r="E98" t="n">
-        <v>7816060.295731476</v>
+        <v>7847665.196937482</v>
       </c>
       <c r="F98" t="n">
-        <v>-4.346771038922388</v>
+        <v>-4.156553228174255</v>
       </c>
       <c r="G98" t="n">
-        <v>0.3841858896809982</v>
+        <v>0.3832745655695799</v>
       </c>
       <c r="H98" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="99">
@@ -3400,19 +3400,19 @@
         <v>21000000</v>
       </c>
       <c r="D99" t="n">
-        <v>36.23416723526778</v>
+        <v>36.46182859254305</v>
       </c>
       <c r="E99" t="n">
-        <v>10347820.05933512</v>
+        <v>10442760.87399487</v>
       </c>
       <c r="F99" t="n">
-        <v>-2.029792248903167</v>
+        <v>-1.744098459040662</v>
       </c>
       <c r="G99" t="n">
-        <v>36.06652763174253</v>
+        <v>36.03383640891963</v>
       </c>
       <c r="H99" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="100">
@@ -3430,19 +3430,19 @@
         <v>223000000</v>
       </c>
       <c r="D100" t="n">
-        <v>3.156797711598248</v>
+        <v>3.182219833676045</v>
       </c>
       <c r="E100" t="n">
-        <v>3683151.047598855</v>
+        <v>3766781.320410729</v>
       </c>
       <c r="F100" t="n">
-        <v>1.391614553951696</v>
+        <v>1.83149482302352</v>
       </c>
       <c r="G100" t="n">
-        <v>3.125286178539979</v>
+        <v>3.128121358251112</v>
       </c>
       <c r="H100" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
     <row r="101">
@@ -3460,19 +3460,19 @@
         <v>100000000</v>
       </c>
       <c r="D101" t="n">
-        <v>15.77405891378906</v>
+        <v>15.880922078181</v>
       </c>
       <c r="E101" t="n">
-        <v>32019059.55696171</v>
+        <v>32715960.2208523</v>
       </c>
       <c r="F101" t="n">
-        <v>-5.884511831169386</v>
+        <v>-5.272966071964917</v>
       </c>
       <c r="G101" t="n">
-        <v>16.19249421208042</v>
+        <v>16.16095663836915</v>
       </c>
       <c r="H101" t="n">
-        <v>1743296428778</v>
+        <v>1743297089423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>